<commit_message>
Fixed some empty cells in WC file header listing
</commit_message>
<xml_diff>
--- a/etuff/FileHeadersWC.xlsx
+++ b/etuff/FileHeadersWC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\tagbase\etuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="121">
   <si>
     <t>csv_suffix</t>
   </si>
@@ -923,6 +923,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H95" totalsRowShown="0">
+  <autoFilter ref="A1:H95"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="csv_suffix"/>
+    <tableColumn id="2" name="column_name"/>
+    <tableColumn id="3" name="description"/>
+    <tableColumn id="4" name="no_longer_used"/>
+    <tableColumn id="5" name="dap_version"/>
+    <tableColumn id="6" name="userguide_version"/>
+    <tableColumn id="7" name="date_first_introduced"/>
+    <tableColumn id="8" name="person_first_introduced"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1190,11 +1207,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="62.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1233,6 +1259,15 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>201903</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1244,6 +1279,15 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>201903</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1255,6 +1299,15 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>201903</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1266,6 +1319,15 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>201903</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1337,6 +1399,15 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>201903</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1408,6 +1479,15 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>201903</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -3051,5 +3131,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>